<commit_message>
Fixed Non Technical skills weightage problem
</commit_message>
<xml_diff>
--- a/Upload-JD/JD_Updated.xlsx
+++ b/Upload-JD/JD_Updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\satish.kumar\deeplearning\resumeranking\ResumeRanking\Upload-JD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saurabh.keshari\NLP\resumeranking\Upload-JD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8229A1A5-91CB-44F4-A301-D8FD4CC0F37B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7454796C-78C6-478D-894C-6C87C1D20EAF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{5A5CFA35-AC6A-4099-A87E-D4FB9658EBAF}"/>
   </bookViews>
@@ -71,19 +71,6 @@
     <t>5-7</t>
   </si>
   <si>
-    <t>JD For Business Analyst
-Sub-Domain58; Core Banking Solution, CASA, Loan, General Ledger, Customer solution.
-1.MBA Preferred (Finance &amp;amp; Banking)
-2.Should have an overall experience of minimum 3-6 years on banking domain in Product/Service Based Company and working as a Business Analyst.
-3.Banking experience is Preferred.
-4.Should have worked on at least one Core Banking Solution. (Ex58; Finacle, Oracle Flexcube, Fiserv, TCS BaNcs, FIS Profile etc.)
-Project Requirement58;
-Mandatory Skill58;
-1.Candidate should have experience in software development methodologies such as waterfall, agile, etc. 
-2.Candidate should have experience in Gathering, analyzing &amp;amp; documenting processes, rules and functions required to support these needs and corresponding requirements.
-3.Experience in interacting with Business users &amp;amp; SME providing recommendations to resolve issues for various business/technical groups &amp;amp; defining strategic solutions to business problems in a multiple p</t>
-  </si>
-  <si>
     <t>Banking &amp; Finance--Master,Banking &amp; Finance--Master</t>
   </si>
   <si>
@@ -224,6 +211,20 @@
   </si>
   <si>
     <t>Banking &amp; Finance--Master java</t>
+  </si>
+  <si>
+    <t>JD For Business Analyst
+Sub-Domain58; Core Banking Solution, CASA, Loan, General Ledger, Customer solution.
+1.MBA Preferred (Finance &amp;amp; Banking)
+2.Should have an overall experience of minimum 3-6 years on banking domain in Product/Service Based Company and working as a Business Analyst.
+3.Banking experience is Preferred.
+4.Should have worked on at least one Core Banking Solution. (Ex58; Finacle, Oracle Flexcube, Fiserv, TCS BaNcs, FIS Profile etc.) 
+communication , team player
+Project Requirement58;
+Mandatory Skill58;
+1.Candidate should have experience in software development methodologies such as waterfall, agile, etc. 
+2.Candidate should have experience in Gathering, analyzing &amp;amp; documenting processes, rules and functions required to support these needs and corresponding requirements.
+3.Experience in interacting with Business users &amp;amp; SME providing recommendations to resolve issues for various business/technical groups &amp;amp; defining strategic solutions to business problems in a multiple p</t>
   </si>
 </sst>
 </file>
@@ -620,7 +621,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,90 +669,90 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -760,67 +761,67 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="270" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
@@ -829,16 +830,16 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>